<commit_message>
spora edycja kodu i pdf
</commit_message>
<xml_diff>
--- a/zad1/double_wartosciBezwzgledne.xlsx
+++ b/zad1/double_wartosciBezwzgledne.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
   <si>
     <t>Wyniki</t>
   </si>
@@ -89,6 +89,850 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pl-PL"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="1600"/>
+              <a:t>Procentowa szansa na lepszy wynik jednego sumowania wzgledem  drugiego</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.16782934530591884"/>
+          <c:y val="9.3403368699133786E-3"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln cap="sq"/>
+      </c:spPr>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>od tylu</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$27:$A$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$27:$C$46</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.67</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.67</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>od przodu</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$27:$A$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$27:$D$46</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.23</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="119342976"/>
+        <c:axId val="119344512"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="119342976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="119344512"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="119344512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="119342976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+      </c:dTable>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pl-PL"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="1400"/>
+              <a:t>Wartość</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="1400" baseline="0"/>
+              <a:t> bezwzględna różnicy sumowań od właściwego wyniku</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL" sz="1400"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>od tyłu</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$27:$A$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$27:$E$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1.2999999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6000000000000001E-17</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1E-17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.3600000000000002E-18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.3000000000000002E-18</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.6999999999999999E-18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.4999999999999999E-18</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.1000000000000002E-19</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.06E-19</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.2000000000000001E-19</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.0999999999999999E-19</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.0999999999999999E-19</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.4999999999999996E-19</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.56E-18</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.8000000000000001E-18</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.3000000000000002E-18</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.4999999999999995E-18</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.13E-17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.6000000000000001E-17</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.38E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>od przodu</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$27:$A$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>-1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$27:$F$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1.2999999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5699999999999999E-16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.97E-16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.59E-16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.03E-16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.7700000000000006E-17</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.9999999999999999E-17</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.15E-17</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.59E-17</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.2399999999999998E-18</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.2490000000000003E-18</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.5799999999999999E-17</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.1700000000000002E-17</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.0258999999999997E-17</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.8000000000000006E-17</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.0350000000000001E-16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.598E-16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.975E-16</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.5699999999999999E-16</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.38E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls/>
+        <c:marker val="1"/>
+        <c:axId val="85337216"/>
+        <c:axId val="85338752"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="85337216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="t"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="85338752"/>
+        <c:crosses val="max"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="85338752"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:max val="1.6000000000000004E-4"/>
+          <c:min val="1.0000000000000011E-20"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="9525">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="85337216"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>66676</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>659424</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>168517</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1663211</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>131884</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 10"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -376,10 +1220,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -819,8 +1663,442 @@
         <v>1.9499999999999999E-3</v>
       </c>
     </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27">
+        <v>-1</v>
+      </c>
+      <c r="B27">
+        <v>-0.9</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.67</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="E27">
+        <v>1.2999999999999999E-5</v>
+      </c>
+      <c r="F27">
+        <v>1.2999999999999999E-5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28">
+        <v>-0.9</v>
+      </c>
+      <c r="B28">
+        <v>-0.8</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0.82</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="E28">
+        <v>1.6000000000000001E-17</v>
+      </c>
+      <c r="F28">
+        <v>2.5699999999999999E-16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29">
+        <v>-0.8</v>
+      </c>
+      <c r="B29">
+        <v>-0.7</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0.79</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="E29">
+        <v>1.1E-17</v>
+      </c>
+      <c r="F29">
+        <v>1.97E-16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30">
+        <v>-0.7</v>
+      </c>
+      <c r="B30">
+        <v>-0.6</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="E30">
+        <v>8.3600000000000002E-18</v>
+      </c>
+      <c r="F30">
+        <v>1.59E-16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31">
+        <v>-0.6</v>
+      </c>
+      <c r="B31">
+        <v>-0.5</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0.72</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="E31">
+        <v>4.3000000000000002E-18</v>
+      </c>
+      <c r="F31">
+        <v>1.03E-16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32">
+        <v>-0.5</v>
+      </c>
+      <c r="B32">
+        <v>-0.4</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0.68</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="E32">
+        <v>2.6999999999999999E-18</v>
+      </c>
+      <c r="F32">
+        <v>5.7700000000000006E-17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33">
+        <v>-0.4</v>
+      </c>
+      <c r="B33">
+        <v>-0.3</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="E33">
+        <v>1.4999999999999999E-18</v>
+      </c>
+      <c r="F33">
+        <v>4.9999999999999999E-17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34">
+        <v>-0.3</v>
+      </c>
+      <c r="B34">
+        <v>-0.2</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0.61</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="E34">
+        <v>8.1000000000000002E-19</v>
+      </c>
+      <c r="F34">
+        <v>3.15E-17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35">
+        <v>-0.2</v>
+      </c>
+      <c r="B35">
+        <v>-0.1</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="E35">
+        <v>4.06E-19</v>
+      </c>
+      <c r="F35">
+        <v>1.59E-17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36">
+        <v>-0.1</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="E36">
+        <v>1.2000000000000001E-19</v>
+      </c>
+      <c r="F36">
+        <v>4.2399999999999998E-18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37">
+        <v>0</v>
+      </c>
+      <c r="B37">
+        <v>0.1</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="E37">
+        <v>1.0999999999999999E-19</v>
+      </c>
+      <c r="F37">
+        <v>4.2490000000000003E-18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38">
+        <v>0.1</v>
+      </c>
+      <c r="B38">
+        <v>0.2</v>
+      </c>
+      <c r="C38" s="2">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="E38">
+        <v>4.0999999999999999E-19</v>
+      </c>
+      <c r="F38">
+        <v>1.5799999999999999E-17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39">
+        <v>0.2</v>
+      </c>
+      <c r="B39">
+        <v>0.3</v>
+      </c>
+      <c r="C39" s="2">
+        <v>0.61</v>
+      </c>
+      <c r="D39" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="E39">
+        <v>7.4999999999999996E-19</v>
+      </c>
+      <c r="F39">
+        <v>3.1700000000000002E-17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40">
+        <v>0.3</v>
+      </c>
+      <c r="B40">
+        <v>0.4</v>
+      </c>
+      <c r="C40" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="D40" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="E40">
+        <v>1.56E-18</v>
+      </c>
+      <c r="F40">
+        <v>5.0258999999999997E-17</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41">
+        <v>0.4</v>
+      </c>
+      <c r="B41">
+        <v>0.5</v>
+      </c>
+      <c r="C41" s="2">
+        <v>0.69</v>
+      </c>
+      <c r="D41" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="E41">
+        <v>2.8000000000000001E-18</v>
+      </c>
+      <c r="F41">
+        <v>5.8000000000000006E-17</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42">
+        <v>0.5</v>
+      </c>
+      <c r="B42">
+        <v>0.6</v>
+      </c>
+      <c r="C42" s="2">
+        <v>0.72</v>
+      </c>
+      <c r="D42" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="E42">
+        <v>4.3000000000000002E-18</v>
+      </c>
+      <c r="F42">
+        <v>1.0350000000000001E-16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43">
+        <v>0.6</v>
+      </c>
+      <c r="B43">
+        <v>0.7</v>
+      </c>
+      <c r="C43" s="2">
+        <v>0.76</v>
+      </c>
+      <c r="D43" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="E43">
+        <v>8.4999999999999995E-18</v>
+      </c>
+      <c r="F43">
+        <v>1.598E-16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44">
+        <v>0.7</v>
+      </c>
+      <c r="B44">
+        <v>0.8</v>
+      </c>
+      <c r="C44" s="2">
+        <v>0.79</v>
+      </c>
+      <c r="D44" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="E44">
+        <v>1.13E-17</v>
+      </c>
+      <c r="F44">
+        <v>1.975E-16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45">
+        <v>0.8</v>
+      </c>
+      <c r="B45">
+        <v>0.9</v>
+      </c>
+      <c r="C45" s="2">
+        <v>0.83</v>
+      </c>
+      <c r="D45" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="E45">
+        <v>1.6000000000000001E-17</v>
+      </c>
+      <c r="F45">
+        <v>2.5699999999999999E-16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46">
+        <v>0.9</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46" s="2">
+        <v>0.67</v>
+      </c>
+      <c r="D46" s="2">
+        <v>0.23</v>
+      </c>
+      <c r="E46">
+        <v>1.38E-5</v>
+      </c>
+      <c r="F46">
+        <v>1.38E-5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>